<commit_message>
geckoderiver.exe is added and edit data of excel sheet
</commit_message>
<xml_diff>
--- a/SWE 2/ST-Comm_Testing/logInData.xlsx
+++ b/SWE 2/ST-Comm_Testing/logInData.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>John</t>
   </si>
@@ -52,10 +51,10 @@
     <t>Jack</t>
   </si>
   <si>
-    <t>'</t>
-  </si>
-  <si>
     <t>Vc123</t>
+  </si>
+  <si>
+    <t>AndrewEmad</t>
   </si>
 </sst>
 </file>
@@ -374,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -407,12 +406,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -434,16 +429,20 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>